<commit_message>
Fixed bug in which tables were not appearing correctly.
</commit_message>
<xml_diff>
--- a/test/files/FQ_BFR5.xlsx
+++ b/test/files/FQ_BFR5.xlsx
@@ -13021,7 +13021,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -13030,17 +13030,17 @@
     <col min="2" max="2" width="14.5" style="75" customWidth="1"/>
     <col min="3" max="3" width="27.1640625" style="75" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="75" customWidth="1"/>
-    <col min="5" max="5" width="45" style="75" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" style="75" customWidth="1"/>
-    <col min="7" max="7" width="45.5" style="75" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" style="75" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" style="75" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="75" customWidth="1"/>
+    <col min="6" max="6" width="14" style="75" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="158" customWidth="1"/>
-    <col min="11" max="11" width="32.33203125" style="75" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5" style="75" customWidth="1"/>
-    <col min="13" max="13" width="28.1640625" style="75" customWidth="1"/>
-    <col min="14" max="14" width="32.5" style="75" customWidth="1"/>
-    <col min="15" max="15" width="26.6640625" style="75" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" style="75" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="75" customWidth="1"/>
     <col min="16" max="16" width="3.5" style="74" customWidth="1"/>
     <col min="17" max="17" width="12" style="75" customWidth="1"/>
     <col min="18" max="18" width="24" style="75" customWidth="1"/>

</xml_diff>